<commit_message>
actualizacion de las hojas
</commit_message>
<xml_diff>
--- a/automatismo.xlsx
+++ b/automatismo.xlsx
@@ -13,6 +13,7 @@
     <sheet name="Detalles" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="INACTIVAS" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="PQ AUSEN" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="PQ CAMION" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -4763,4 +4764,223 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>FECHA SCAN PET</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>CEDULA TECNICO</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">NOMBRE TECNICO </t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Centro de costos</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>OBSERVACIÓN</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Cargo colaborador</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="n">
+        <v>45414</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1022355666</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>JUAN DAVID BECERRA PEÑA</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>1197001 - Aprovisionamiento FTTH C-CW5903-23 BOG</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>TECNICO II / INSTALADOR FTTH</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="n">
+        <v>45414</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1006886735</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>WILBERTO DARIO PEREZ TILLER</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>1197001 - Aprovisionamiento FTTH C-CW5903-23 BOG</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>TECNICO II / INSTALADOR FTTH</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="n">
+        <v>45415</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1022355666</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>JUAN DAVID BECERRA PEÑA</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>1197001 - Aprovisionamiento FTTH C-CW5903-23 BOG</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>TECNICO II / INSTALADOR FTTH</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="n">
+        <v>45416</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1006886735</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>WILBERTO DARIO PEREZ TILLER</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>1197001 - Aprovisionamiento FTTH C-CW5903-23 BOG</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>TECNICO II / INSTALADOR FTTH</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="n">
+        <v>45416</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1022355666</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>JUAN DAVID BECERRA PEÑA</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>1197001 - Aprovisionamiento FTTH C-CW5903-23 BOG</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>TECNICO II / INSTALADOR FTTH</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="n">
+        <v>45418</v>
+      </c>
+      <c r="B7" t="n">
+        <v>1022355666</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>JUAN DAVID BECERRA PEÑA</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>1197001 - Aprovisionamiento FTTH C-CW5903-23 BOG</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>TECNICO II / INSTALADOR FTTH</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="n">
+        <v>45419</v>
+      </c>
+      <c r="B8" t="n">
+        <v>1022355666</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>JUAN DAVID BECERRA PEÑA</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>1197001 - Aprovisionamiento FTTH C-CW5903-23 BOG</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>TECNICO II / INSTALADOR FTTH</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>